<commit_message>
changed the input excels for scenarios for D5.2 in NewTrends. Only buildings are missing
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Battery.xlsx
+++ b/data/input_operation/OperationScenario_Component_Battery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ED946A5-C157-4AA2-BA45-BB34AF45AC0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BD1574-7013-46F8-BE4A-BE39A7F37200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bat" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -892,10 +892,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -933,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
operation input tables updated
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Battery.xlsx
+++ b/data/input_operation/OperationScenario_Component_Battery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/Flex/data/input_operation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950C2CA7-89E6-CB49-9623-B31DA86FDABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BD1574-7013-46F8-BE4A-BE39A7F37200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19200" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bat" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>ID_Battery</t>
   </si>
@@ -540,48 +540,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -597,7 +597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -893,15 +893,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -956,6 +956,35 @@
         <v>4500</v>
       </c>
       <c r="I2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>0.95</v>
+      </c>
+      <c r="E3">
+        <v>4500</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>0.95</v>
+      </c>
+      <c r="H3">
+        <v>4500</v>
+      </c>
+      <c r="I3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
input data back to original for the validation
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Battery.xlsx
+++ b/data/input_operation/OperationScenario_Component_Battery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E325CFB-2D1A-4ABE-8A80-0889783D87D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915629FF-D68D-4FCA-BE58-F419AD2F5DBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bat" sheetId="1" r:id="rId1"/>
@@ -896,12 +896,21 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,7 +939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
scenario setup (energy price tbd)
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Battery.xlsx
+++ b/data/input_operation/OperationScenario_Component_Battery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BD1574-7013-46F8-BE4A-BE39A7F37200}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE812E33-CE0A-F944-ABC8-F5A9B211E429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2880" yWindow="-20720" windowWidth="23580" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bat" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>ID_Battery</t>
   </si>
@@ -540,48 +540,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -597,7 +597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -893,15 +893,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="182" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,12 +930,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7000</v>
+        <v>20000</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -959,12 +959,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -985,6 +985,93 @@
         <v>4500</v>
       </c>
       <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>0.95</v>
+      </c>
+      <c r="E4">
+        <v>4500</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>0.95</v>
+      </c>
+      <c r="H4">
+        <v>4500</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0.95</v>
+      </c>
+      <c r="E5">
+        <v>4500</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0.95</v>
+      </c>
+      <c r="H5">
+        <v>4500</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>0.95</v>
+      </c>
+      <c r="E6">
+        <v>4500</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>0.95</v>
+      </c>
+      <c r="H6">
+        <v>4500</v>
+      </c>
+      <c r="I6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>